<commit_message>
Post SIT Cybersource Vietin & 7Eleven
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Cybersourcepaymaya/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Cybersourcepaymaya/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\Kalyana\Traveloka_DataAutomation_Portal_Cybersourcevietin\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Portal_Cybersourcepaymaya\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C172C6-097D-4C48-8B9A-22A66D46A904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F12CA58-338F-434E-B169-1F7C16BF1DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="1236" windowWidth="17280" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -239,7 +239,7 @@
     <t>RPA021_MOLPAY_Captcha_SiteKey</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_Cred_Gmail</t>
+    <t>RPA_Moon_Cred_Gmail</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>

</xml_diff>